<commit_message>
tons of updates for items, including dbcs and client patches
</commit_message>
<xml_diff>
--- a/Custom/Custom Items/DBC edit/Item/Excel for bringing changes.xlsx
+++ b/Custom/Custom Items/DBC edit/Item/Excel for bringing changes.xlsx
@@ -1,6 +1,49 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Desktop\WoW Server\Azeroth Fork\DarkChaos-255\Custom\Custom Items\DBC edit\Item\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF6E07F5-A5A5-4F47-9A62-60A4D6253E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{66F4A637-4390-43EE-838E-A013EF500C09}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="DBC base" sheetId="2" r:id="rId2"/>
+    <sheet name="Customs" sheetId="3" r:id="rId3"/>
+    <sheet name="Additions" sheetId="5" r:id="rId4"/>
+  </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DBC base'!$A$1:$H$46097</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
+</workbook>
+</file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>entry</t>
   </si>
@@ -27,6 +70,12 @@
   </si>
   <si>
     <t>SheatheType</t>
+  </si>
+  <si>
+    <t>T12 Waffen</t>
+  </si>
+  <si>
+    <t>T11 Waffen</t>
   </si>
 </sst>
 </file>
@@ -82,9 +131,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -122,7 +171,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -228,7 +277,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -370,10 +419,686 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2F3549-0290-412A-A4EA-6316F7685783}">
+  <dimension ref="A1:C59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>50603</v>
+      </c>
+      <c r="B2">
+        <v>91000</v>
+      </c>
+      <c r="C2">
+        <v>91100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>50608</v>
+      </c>
+      <c r="B3">
+        <v>91001</v>
+      </c>
+      <c r="C3">
+        <v>91101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>50621</v>
+      </c>
+      <c r="B4">
+        <v>91002</v>
+      </c>
+      <c r="C4">
+        <v>91102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>50631</v>
+      </c>
+      <c r="B5">
+        <v>91003</v>
+      </c>
+      <c r="C5">
+        <v>91103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>50638</v>
+      </c>
+      <c r="B6">
+        <v>91004</v>
+      </c>
+      <c r="C6">
+        <v>91104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>50641</v>
+      </c>
+      <c r="B7">
+        <v>91005</v>
+      </c>
+      <c r="C7">
+        <v>91105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>50648</v>
+      </c>
+      <c r="B8">
+        <v>91006</v>
+      </c>
+      <c r="C8">
+        <v>91106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>50654</v>
+      </c>
+      <c r="B9">
+        <v>91007</v>
+      </c>
+      <c r="C9">
+        <v>91107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>50672</v>
+      </c>
+      <c r="B10">
+        <v>91008</v>
+      </c>
+      <c r="C10">
+        <v>91108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>50676</v>
+      </c>
+      <c r="B11">
+        <v>91009</v>
+      </c>
+      <c r="C11">
+        <v>91109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>50684</v>
+      </c>
+      <c r="B12">
+        <v>91010</v>
+      </c>
+      <c r="C12">
+        <v>91110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>50685</v>
+      </c>
+      <c r="B13">
+        <v>91011</v>
+      </c>
+      <c r="C13">
+        <v>91111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>50692</v>
+      </c>
+      <c r="B14">
+        <v>91012</v>
+      </c>
+      <c r="C14">
+        <v>91112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>50695</v>
+      </c>
+      <c r="B15">
+        <v>91013</v>
+      </c>
+      <c r="C15">
+        <v>91113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>50704</v>
+      </c>
+      <c r="B16">
+        <v>91014</v>
+      </c>
+      <c r="C16">
+        <v>91114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>50708</v>
+      </c>
+      <c r="B17">
+        <v>91015</v>
+      </c>
+      <c r="C17">
+        <v>91115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>50709</v>
+      </c>
+      <c r="B18">
+        <v>91016</v>
+      </c>
+      <c r="C18">
+        <v>91116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>50710</v>
+      </c>
+      <c r="B19">
+        <v>91017</v>
+      </c>
+      <c r="C19">
+        <v>91117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>50725</v>
+      </c>
+      <c r="B20">
+        <v>91018</v>
+      </c>
+      <c r="C20">
+        <v>91118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>50727</v>
+      </c>
+      <c r="B21">
+        <v>91019</v>
+      </c>
+      <c r="C21">
+        <v>91119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>51389</v>
+      </c>
+      <c r="B22">
+        <v>91020</v>
+      </c>
+      <c r="C22">
+        <v>91120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>51391</v>
+      </c>
+      <c r="B23">
+        <v>91021</v>
+      </c>
+      <c r="C23">
+        <v>91121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>51393</v>
+      </c>
+      <c r="B24">
+        <v>91022</v>
+      </c>
+      <c r="C24">
+        <v>91122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>51395</v>
+      </c>
+      <c r="B25">
+        <v>91023</v>
+      </c>
+      <c r="C25">
+        <v>91123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>51398</v>
+      </c>
+      <c r="B26">
+        <v>91024</v>
+      </c>
+      <c r="C26">
+        <v>91124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>51399</v>
+      </c>
+      <c r="B27">
+        <v>91025</v>
+      </c>
+      <c r="C27">
+        <v>91125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>51401</v>
+      </c>
+      <c r="B28">
+        <v>91026</v>
+      </c>
+      <c r="C28">
+        <v>91126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>51403</v>
+      </c>
+      <c r="B29">
+        <v>91027</v>
+      </c>
+      <c r="C29">
+        <v>91127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>51405</v>
+      </c>
+      <c r="B30">
+        <v>91028</v>
+      </c>
+      <c r="C30">
+        <v>91128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>51412</v>
+      </c>
+      <c r="B31">
+        <v>91029</v>
+      </c>
+      <c r="C31">
+        <v>91129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>51432</v>
+      </c>
+      <c r="B32">
+        <v>91030</v>
+      </c>
+      <c r="C32">
+        <v>91130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>51440</v>
+      </c>
+      <c r="B33">
+        <v>91031</v>
+      </c>
+      <c r="C33">
+        <v>91131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>51442</v>
+      </c>
+      <c r="B34">
+        <v>91032</v>
+      </c>
+      <c r="C34">
+        <v>91132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>51444</v>
+      </c>
+      <c r="B35">
+        <v>91033</v>
+      </c>
+      <c r="C35">
+        <v>91133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>51446</v>
+      </c>
+      <c r="B36">
+        <v>91034</v>
+      </c>
+      <c r="C36">
+        <v>91134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>51448</v>
+      </c>
+      <c r="B37">
+        <v>91035</v>
+      </c>
+      <c r="C37">
+        <v>91135</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>51450</v>
+      </c>
+      <c r="B38">
+        <v>91036</v>
+      </c>
+      <c r="C38">
+        <v>91136</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>51454</v>
+      </c>
+      <c r="B39">
+        <v>91037</v>
+      </c>
+      <c r="C39">
+        <v>91137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>51457</v>
+      </c>
+      <c r="B40">
+        <v>91038</v>
+      </c>
+      <c r="C40">
+        <v>91138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>51481</v>
+      </c>
+      <c r="B41">
+        <v>91039</v>
+      </c>
+      <c r="C41">
+        <v>91139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>51516</v>
+      </c>
+      <c r="B42">
+        <v>91040</v>
+      </c>
+      <c r="C42">
+        <v>91140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>51518</v>
+      </c>
+      <c r="B43">
+        <v>91041</v>
+      </c>
+      <c r="C43">
+        <v>91141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>51520</v>
+      </c>
+      <c r="B44">
+        <v>91042</v>
+      </c>
+      <c r="C44">
+        <v>91142</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>51522</v>
+      </c>
+      <c r="B45">
+        <v>91043</v>
+      </c>
+      <c r="C45">
+        <v>91143</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>51524</v>
+      </c>
+      <c r="B46">
+        <v>91044</v>
+      </c>
+      <c r="C46">
+        <v>91144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>51526</v>
+      </c>
+      <c r="B47">
+        <v>91045</v>
+      </c>
+      <c r="C47">
+        <v>91145</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>51528</v>
+      </c>
+      <c r="B48">
+        <v>91046</v>
+      </c>
+      <c r="C48">
+        <v>91146</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>51529</v>
+      </c>
+      <c r="B49">
+        <v>91047</v>
+      </c>
+      <c r="C49">
+        <v>91147</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>49623</v>
+      </c>
+      <c r="B50">
+        <v>91048</v>
+      </c>
+      <c r="C50">
+        <v>91148</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>50730</v>
+      </c>
+      <c r="B51">
+        <v>91049</v>
+      </c>
+      <c r="C51">
+        <v>91149</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>50731</v>
+      </c>
+      <c r="B52">
+        <v>91050</v>
+      </c>
+      <c r="C52">
+        <v>91150</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>50732</v>
+      </c>
+      <c r="B53">
+        <v>91051</v>
+      </c>
+      <c r="C53">
+        <v>91151</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>50733</v>
+      </c>
+      <c r="B54">
+        <v>91052</v>
+      </c>
+      <c r="C54">
+        <v>91152</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>50734</v>
+      </c>
+      <c r="B55">
+        <v>91053</v>
+      </c>
+      <c r="C55">
+        <v>91153</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>50735</v>
+      </c>
+      <c r="B56">
+        <v>91054</v>
+      </c>
+      <c r="C56">
+        <v>91154</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>50736</v>
+      </c>
+      <c r="B57">
+        <v>91055</v>
+      </c>
+      <c r="C57">
+        <v>91155</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>50737</v>
+      </c>
+      <c r="B58">
+        <v>91056</v>
+      </c>
+      <c r="C58">
+        <v>91156</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>50738</v>
+      </c>
+      <c r="B59">
+        <v>91057</v>
+      </c>
+      <c r="C59">
+        <v>91157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1929,7 +2654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4003EDA7-8065-44A6-AE99-60B9BC8F979A}">
   <dimension ref="A1:H117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+    <sheetView topLeftCell="A62" workbookViewId="0">
       <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>

</xml_diff>